<commit_message>
Mudança no arquivo de persistência e ateração na planilha (que eu tinha esquecido de alterar
</commit_message>
<xml_diff>
--- a/Documentos/Tarefas.xlsx
+++ b/Documentos/Tarefas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t xml:space="preserve">Tarefa</t>
   </si>
@@ -55,7 +55,7 @@
     <t xml:space="preserve">Tiago</t>
   </si>
   <si>
-    <t xml:space="preserve">Fase final de implementação</t>
+    <t xml:space="preserve">Aguarda testes</t>
   </si>
   <si>
     <t xml:space="preserve">Algortimo de Dijkstra para definir o menor caminho a ser percorrido entre o vértice do indivíduo e o vértice do ponto de encontro</t>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t xml:space="preserve">Depende da tarefa de criar telas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementação do algoritmo de Dijkstra com retorno de distâcia de vertices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iniciado</t>
   </si>
 </sst>
 </file>
@@ -189,20 +195,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="119.546558704453"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.1012145748988"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="120.615384615385"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.3157894736842"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -318,6 +324,17 @@
       </c>
       <c r="D9" s="0" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alteração da planilha; Criação do método para ler valores no arquivo .txt
</commit_message>
<xml_diff>
--- a/Documentos/Tarefas.xlsx
+++ b/Documentos/Tarefas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t xml:space="preserve">Tarefa</t>
   </si>
@@ -46,22 +46,25 @@
     <t xml:space="preserve">Douglas</t>
   </si>
   <si>
+    <t xml:space="preserve">Em desenvolvimento…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algoritmo de floyd warshall para definir matriz de custo de todos os vértices para todos os vértices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aguarda testes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algortimo de Dijkstra para definir o menor caminho a ser percorrido entre o vértice do indivíduo e o vértice do ponto de encontro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ivens</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aguardando início</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Algoritmo de floyd warshall para definir matriz de custo de todos os vértices para todos os vértices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiago</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aguarda testes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Algortimo de Dijkstra para definir o menor caminho a ser percorrido entre o vértice do indivíduo e o vértice do ponto de encontro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ivens</t>
   </si>
   <si>
     <t xml:space="preserve">Revisar documento de requisitos</t>
@@ -99,7 +102,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D/M/YYYY"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -122,6 +125,14 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -165,17 +176,33 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -195,148 +222,177 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="120.615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.3157894736842"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.6437246963563"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0971659919028"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8097165991903"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.5303643724696"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.3805668016194"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.1943319838057"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="5" t="n">
         <v>43201</v>
       </c>
+      <c r="D2" s="6"/>
       <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="5" t="n">
         <v>43201</v>
       </c>
+      <c r="D3" s="6"/>
       <c r="E3" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" customFormat="false" ht="41.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="5" t="n">
         <v>43201</v>
       </c>
+      <c r="D4" s="6"/>
       <c r="E4" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="0" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5" t="n">
         <v>43201</v>
       </c>
+      <c r="D5" s="6"/>
       <c r="E5" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="5" t="n">
         <v>43201</v>
       </c>
+      <c r="D6" s="6"/>
       <c r="E6" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>17</v>
-      </c>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>18</v>
-      </c>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="0" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
       <c r="E10" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Correção de bug classe operadorArquivos; realização de testes; atualização da planilha; atualização do arquivo padrão .txt
</commit_message>
<xml_diff>
--- a/Documentos/Tarefas.xlsx
+++ b/Documentos/Tarefas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t xml:space="preserve">Tarefa</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t xml:space="preserve">Iniciado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criar verificação na leitura dos valores das arestas onde não pode ser negativa</t>
   </si>
 </sst>
 </file>
@@ -222,20 +225,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="59.6437246963563"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0971659919028"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8097165991903"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.5303643724696"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.3805668016194"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.1943319838057"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.2024291497976"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.995951417004"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -380,7 +383,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="35.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
o cavalo esqueceu de salvar a planilha
</commit_message>
<xml_diff>
--- a/Documentos/Tarefas.xlsx
+++ b/Documentos/Tarefas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t xml:space="preserve">Tarefa</t>
   </si>
@@ -46,7 +46,10 @@
     <t xml:space="preserve">Douglas</t>
   </si>
   <si>
-    <t xml:space="preserve">Em desenvolvimento…</t>
+    <t xml:space="preserve">entregue dentro do prazo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">correção de bugs</t>
   </si>
   <si>
     <t xml:space="preserve">Algoritmo de floyd warshall para definir matriz de custo de todos os vértices para todos os vértices</t>
@@ -64,15 +67,18 @@
     <t xml:space="preserve">Ivens</t>
   </si>
   <si>
+    <t xml:space="preserve">finalizado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisar documento de requisitos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lilian</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aguardando início</t>
   </si>
   <si>
-    <t xml:space="preserve">Revisar documento de requisitos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lilian</t>
-  </si>
-  <si>
     <t xml:space="preserve">Revisar diagrama de classes</t>
   </si>
   <si>
@@ -88,22 +94,23 @@
     <t xml:space="preserve">Depende da tarefa de criar telas</t>
   </si>
   <si>
-    <t xml:space="preserve">Implementação do algoritmo de Dijkstra com retorno de distâcia de vertices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iniciado</t>
-  </si>
-  <si>
     <t xml:space="preserve">Criar verificação na leitura dos valores das arestas onde não pode ser negativa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementar escolha de direção da aresta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arquivos com grafos para teste</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D/M/YYYY"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -179,7 +186,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -204,8 +211,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -225,20 +240,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.2024291497976"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.995951417004"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.7449392712551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.7368421052632"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.0647773279352"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -273,136 +288,143 @@
       <c r="C2" s="5" t="n">
         <v>43201</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="E2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="5" t="n">
         <v>43201</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="E3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="41.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="5" t="n">
         <v>43201</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="0" t="s">
-        <v>14</v>
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>43201</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="4"/>
       <c r="E5" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>43201</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="4"/>
       <c r="E6" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="6"/>
+      <c r="D8" s="4"/>
       <c r="E8" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="6"/>
+        <v>22</v>
+      </c>
+      <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="35.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="35.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C10" s="6" t="n">
+        <v>43208</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="n">
+        <v>43208</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="8" t="n">
+        <v>43208</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Correção da leitura de valores negativos nas arestas; Criado o método para escrever em arquivo .txt; Correção da classe Indivíduo;
</commit_message>
<xml_diff>
--- a/Documentos/Tarefas.xlsx
+++ b/Documentos/Tarefas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t xml:space="preserve">Tarefa</t>
   </si>
@@ -107,10 +107,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D/M/YYYY"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -186,7 +187,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -211,7 +212,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -243,17 +252,17 @@
   <dimension ref="A1:G65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6:D8"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.7368421052632"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.2105263157895"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.0647773279352"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.0202429149798"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.3846153846154"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -294,8 +303,9 @@
       <c r="E2" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" customFormat="false" ht="53.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -311,8 +321,9 @@
       <c r="E3" s="0" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="41.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" customFormat="false" ht="50.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -328,6 +339,7 @@
       <c r="E4" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
@@ -343,6 +355,7 @@
       <c r="E5" s="0" t="s">
         <v>18</v>
       </c>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
@@ -358,6 +371,7 @@
       <c r="E6" s="0" t="s">
         <v>18</v>
       </c>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
@@ -369,6 +383,7 @@
       <c r="E7" s="0" t="s">
         <v>18</v>
       </c>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
@@ -380,6 +395,7 @@
       <c r="E8" s="0" t="s">
         <v>18</v>
       </c>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
@@ -390,39 +406,51 @@
       <c r="D9" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="35.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="47.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="6" t="n">
+      <c r="C10" s="7" t="n">
         <v>43208</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="8" t="n">
+        <v>43204</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="6" t="n">
+      <c r="C11" s="7" t="n">
         <v>43208</v>
       </c>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="8" t="n">
+      <c r="C12" s="10" t="n">
         <v>43208</v>
       </c>
+      <c r="F12" s="6"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
Removi o documento de tarefas em formato ODS. Deve ficar só no formato de xlsx
</commit_message>
<xml_diff>
--- a/Documentos/Tarefas.xlsx
+++ b/Documentos/Tarefas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Engenharia de Software\Disciplinas\5º Semestre\Projeto Integrador II\Projeto Xablau\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F913DE2-55FE-4D27-BDF4-EA9BB4971805}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6368A6-D4B8-406B-90F5-916BD0B7AABA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>Tarefa</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>arquivos com grafos para teste</t>
+  </si>
+  <si>
+    <t>Pronto</t>
   </si>
 </sst>
 </file>
@@ -503,7 +506,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,6 +718,9 @@
       <c r="C12" s="10">
         <v>43208</v>
       </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
       <c r="F12" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alterei o diagrama de classes, documento de requisitos, planilha de tarefas e o código fonte. No código fonte, coloquei a Classe OperadorGrafo no pacote de controller, criei um fonte pro Algoritmo de Floyd Warshall e o deixei no pacote de utilitários. Agora a classe do OperadorGrafo somente chama as classes do Dijkstra e do FloydWarshall, assim o código fica mais separado, facilitando a manutenção.
</commit_message>
<xml_diff>
--- a/Documentos/Tarefas.xlsx
+++ b/Documentos/Tarefas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Engenharia de Software\Disciplinas\5º Semestre\Projeto Integrador II\Projeto Xablau\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1B2E2B-983C-44C2-B74F-BE50DB28A00E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD981B1-5598-4B18-B6FB-76365FC0BF9D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>Tarefa</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Ivens, Douglas, Tiago</t>
+  </si>
+  <si>
+    <t>Entregue dentro do prazo</t>
+  </si>
+  <si>
+    <t>Desistiu</t>
   </si>
 </sst>
 </file>
@@ -165,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -201,6 +207,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,7 +632,7 @@
       </c>
       <c r="D5" s="4"/>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="F5" s="6"/>
     </row>
@@ -641,7 +648,7 @@
       </c>
       <c r="D6" s="4"/>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="F6" s="6"/>
     </row>
@@ -745,8 +752,14 @@
       <c r="C13" s="12">
         <v>43215</v>
       </c>
+      <c r="D13" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="E13" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="F13" s="13">
+        <v>43214</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -758,6 +771,28 @@
       </c>
       <c r="C14" s="12">
         <v>43215</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="13">
+        <v>43222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="13">
+        <v>43222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização da Planilha de tarefas; Pequenas alterações nas telas
</commit_message>
<xml_diff>
--- a/Documentos/Tarefas.xlsx
+++ b/Documentos/Tarefas.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Engenharia de Software\Disciplinas\5º Semestre\Projeto Integrador II\Projeto-Xablau\ProjetoXablau\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dougl\Documents\Repositórios\Github\ProjetoXablau\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC0BEF6-5100-4CFD-9D8C-EBDED2CF93B3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
   <si>
     <t>Tarefa</t>
   </si>
@@ -136,12 +135,18 @@
   </si>
   <si>
     <t>Aguardando Pendência</t>
+  </si>
+  <si>
+    <t>Começar o artigo científico</t>
+  </si>
+  <si>
+    <t>Criar tela de tutorial</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
@@ -766,11 +771,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="B20:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,7 +783,7 @@
     <col min="1" max="1" width="40"/>
     <col min="2" max="2" width="19.7109375" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.42578125"/>
-    <col min="4" max="4" width="31.42578125" style="16"/>
+    <col min="4" max="4" width="45" style="16" customWidth="1"/>
     <col min="5" max="5" width="22.7109375"/>
     <col min="6" max="6" width="17.5703125" style="16"/>
     <col min="7" max="1025" width="8.5703125"/>
@@ -1084,6 +1089,28 @@
         <v>43243</v>
       </c>
     </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="7">
+        <v>43257</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="7">
+        <v>43250</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização da Planilha; Iniciado a tela de tutorial
</commit_message>
<xml_diff>
--- a/Documentos/Tarefas.xlsx
+++ b/Documentos/Tarefas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
   <si>
     <t>Tarefa</t>
   </si>
@@ -137,10 +137,16 @@
     <t>Aguardando Pendência</t>
   </si>
   <si>
-    <t>Começar o artigo científico</t>
-  </si>
-  <si>
     <t>Criar tela de tutorial</t>
+  </si>
+  <si>
+    <t>Criar movimentação dos individuos</t>
+  </si>
+  <si>
+    <t>Começar o PDF de explicação</t>
+  </si>
+  <si>
+    <t>Douglas/Tiago/Ivens</t>
   </si>
 </sst>
 </file>
@@ -362,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -458,6 +464,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -772,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="B20:C20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,10 +1100,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="C19" s="7">
         <v>43257</v>
@@ -1102,12 +1111,23 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="7">
+        <v>43250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="35">
         <v>43250</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Concluído a tela 'TelaTutorial'; Concluído a edição de imagens para a TelaTutorial; Atualização da Planilha; Alteração do template padrão SBC para a elaboração do relatório do projeto
</commit_message>
<xml_diff>
--- a/Documentos/Tarefas.xlsx
+++ b/Documentos/Tarefas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
   <si>
     <t>Tarefa</t>
   </si>
@@ -368,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -465,6 +465,12 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -784,7 +790,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E20" sqref="E20:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,6 +1125,12 @@
       <c r="C20" s="7">
         <v>43250</v>
       </c>
+      <c r="E20" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="37">
+        <v>43244</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">

</xml_diff>

<commit_message>
Alteração na tela do mapa, no modelo do Nó e descrição do Dijkstra
Foi realizada alteração no mapa, para realizar-se o desenho do mapa, para melhorar a navegabilidade na tela. Também foi alterado o Nó, para que em vez de trabalhar com vértices, trabalhe com Aresta, para que na Lista encadeada do caminho, seja mais fácil realizar os cálculos para movimentação do indivíduo. Também descrevi o Dijkstra no relatório em template do Latex.
</commit_message>
<xml_diff>
--- a/Documentos/Tarefas.xlsx
+++ b/Documentos/Tarefas.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dougl\Documents\Repositórios\Github\ProjetoXablau\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Engenharia de Software\Disciplinas\5º Semestre\Projeto Integrador II\Projeto-Xablau\ProjetoXablau\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAEEEF4-FE49-4D0F-8760-8F3A3D2DFEC5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
   <si>
     <t>Tarefa</t>
   </si>
@@ -131,12 +132,6 @@
     <t>la de calcular os pontos da curva</t>
   </si>
   <si>
-    <t>Falta verificar como vai ficar o desenho do mapa</t>
-  </si>
-  <si>
-    <t>Aguardando Pendência</t>
-  </si>
-  <si>
     <t>Criar tela de tutorial</t>
   </si>
   <si>
@@ -147,12 +142,21 @@
   </si>
   <si>
     <t>Douglas/Tiago/Ivens</t>
+  </si>
+  <si>
+    <t>Antes da entrega</t>
+  </si>
+  <si>
+    <t>Alteração na lista caminho para ser por aresta</t>
+  </si>
+  <si>
+    <t>Entregue dentro do prazo / houve alterações depois</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
@@ -368,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -473,6 +477,8 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,11 +792,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20:F20"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,7 +804,7 @@
     <col min="1" max="1" width="40"/>
     <col min="2" max="2" width="19.7109375" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.42578125"/>
-    <col min="4" max="4" width="45" style="16" customWidth="1"/>
+    <col min="4" max="4" width="48" style="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.7109375"/>
     <col min="6" max="6" width="17.5703125" style="16"/>
     <col min="7" max="1025" width="8.5703125"/>
@@ -1052,8 +1058,8 @@
       <c r="B15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="7">
-        <v>43222</v>
+      <c r="C15" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="9"/>
@@ -1066,8 +1072,8 @@
       <c r="B16" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="7">
-        <v>43222</v>
+      <c r="C16" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="9"/>
@@ -1084,10 +1090,10 @@
         <v>43243</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" t="s">
-        <v>36</v>
+        <v>41</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>26</v>
       </c>
       <c r="F17" s="34">
         <v>43242</v>
@@ -1103,13 +1109,14 @@
       <c r="C18" s="7">
         <v>43243</v>
       </c>
+      <c r="E18" s="39"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" s="7">
         <v>43257</v>
@@ -1117,7 +1124,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>7</v>
@@ -1134,13 +1141,33 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C21" s="35">
         <v>43250</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="38">
+        <v>43250</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="34">
+        <v>43248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alterações no mapa para o desenho ficar correto e alterações no retorno da lista de caminho
Foi alterado o retorno da lista de caminho para sempre retornar as arestas da maneira correta (Origem -> Destino). Também foram feitas alterações no controller do mapa, no mapa, e em alguns models para que o desenho do mapa fique certo a partir de um arquivo texto.
</commit_message>
<xml_diff>
--- a/Documentos/Tarefas.xlsx
+++ b/Documentos/Tarefas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Engenharia de Software\Disciplinas\5º Semestre\Projeto Integrador II\Projeto-Xablau\ProjetoXablau\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAEEEF4-FE49-4D0F-8760-8F3A3D2DFEC5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172E4232-41CF-4B5F-99CB-4FA239518245}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="46">
   <si>
     <t>Tarefa</t>
   </si>
@@ -151,6 +151,18 @@
   </si>
   <si>
     <t>Entregue dentro do prazo / houve alterações depois</t>
+  </si>
+  <si>
+    <t>Alterar arestas para origem e destino ficar na ordem quando trazer a lista do caminho</t>
+  </si>
+  <si>
+    <t>Mostrar mensagem usuário de erro ao carregar arquivo</t>
+  </si>
+  <si>
+    <t>Corrigir erro ao carregar mapa</t>
+  </si>
+  <si>
+    <t>Diagrama de casos de uso</t>
   </si>
 </sst>
 </file>
@@ -793,10 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,6 +1182,77 @@
         <v>43248</v>
       </c>
     </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="38">
+        <v>43261</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="34">
+        <v>43261</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="38">
+        <v>43261</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="34">
+        <v>43261</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="38">
+        <v>43261</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="34">
+        <v>43261</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="38">
+        <v>43264</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Acerto do individuo que anda pela curva
</commit_message>
<xml_diff>
--- a/Documentos/Tarefas.xlsx
+++ b/Documentos/Tarefas.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Engenharia de Software\GitHub\ProjetoXablau\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10516125940\Documents\GitHub\ProjetoXablau\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A06E44-658A-4BFD-91CB-F17448BCAF86}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="47">
   <si>
     <t>Tarefa</t>
   </si>
@@ -163,12 +162,15 @@
   </si>
   <si>
     <t>Diagrama de casos de uso</t>
+  </si>
+  <si>
+    <t>Corrigir bugs nos individuos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
@@ -804,11 +806,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,6 +1245,14 @@
         <v>43264</v>
       </c>
     </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Alterado os valores do arquivo texto padrão; correção no documento de requisitos; correção no diagrama de casos de uso
</commit_message>
<xml_diff>
--- a/Documentos/Tarefas.xlsx
+++ b/Documentos/Tarefas.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10516125940\Documents\GitHub\ProjetoXablau\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Douglas\Documents\Repositórios\GitHub\ProjetoXablau\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
   <si>
     <t>Tarefa</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Tiago</t>
   </si>
   <si>
-    <t>Aguarda testes</t>
-  </si>
-  <si>
     <t>Algortimo de Dijkstra para definir o menor caminho a ser percorrido entre o vértice do indivíduo e o vértice do ponto de encontro</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
     <t>Concluido</t>
   </si>
   <si>
-    <t>implementando...</t>
-  </si>
-  <si>
     <t>la de calcular os pontos da curva</t>
   </si>
   <si>
@@ -165,6 +159,9 @@
   </si>
   <si>
     <t>Corrigir bugs nos individuos</t>
+  </si>
+  <si>
+    <t>Iniciado</t>
   </si>
 </sst>
 </file>
@@ -175,7 +172,7 @@
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -220,6 +217,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -386,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -395,9 +399,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -451,9 +452,6 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -476,23 +474,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -809,447 +811,459 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40"/>
-    <col min="2" max="2" width="19.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125"/>
-    <col min="4" max="4" width="48" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="8"/>
+    <col min="4" max="4" width="48" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.7109375"/>
-    <col min="6" max="6" width="17.5703125" style="16"/>
+    <col min="6" max="6" width="17.5703125" style="15"/>
     <col min="7" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="30" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="23" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="3">
         <v>43201</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="27">
+      <c r="E2" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="25">
         <v>43201</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>43201</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="22">
+        <v>43201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="23">
-        <v>43201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="B4" s="10" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>13</v>
       </c>
       <c r="C4" s="3">
         <v>43201</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="16">
+        <v>43201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="17">
-        <v>43201</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="B5" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>16</v>
       </c>
       <c r="C5" s="3">
         <v>43201</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="18"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="17"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>16</v>
+      <c r="A6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="C6" s="3">
         <v>43201</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="9" t="s">
+      <c r="D6" s="13"/>
+      <c r="E6" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="17"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4">
+        <v>43208</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="18">
+        <v>43204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="4">
+        <v>43208</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="19">
+        <v>43207</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="5">
+        <v>43208</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="17"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6">
+        <v>43215</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="20">
+        <v>43214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="6">
+        <v>43215</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="20">
+        <v>43268</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="6">
+        <v>43243</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="31">
+        <v>43242</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="6">
+        <v>43243</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="6">
+        <v>43257</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="18"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="11" t="s">
+      <c r="B19" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="18"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="18"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="18"/>
-    </row>
-    <row r="10" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="11" t="s">
+      <c r="C19" s="6">
+        <v>43250</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="33">
+        <v>43244</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="32">
+        <v>43250</v>
+      </c>
+      <c r="E20" s="37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="6">
+        <v>43250</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="31">
+        <v>43248</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="6">
+        <v>43261</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="31">
+        <v>43261</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="6">
+        <v>43261</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="31">
+        <v>43261</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="6">
+        <v>43261</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="31">
+        <v>43261</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="5">
-        <v>43208</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="19">
-        <v>43204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="5">
-        <v>43208</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="20">
-        <v>43207</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="6">
-        <v>43208</v>
-      </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="18"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="7">
-        <v>43215</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="21">
-        <v>43214</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="7">
-        <v>43215</v>
-      </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="15"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="21">
-        <v>43268</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="7">
-        <v>43243</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="34">
-        <v>43242</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="7">
-        <v>43243</v>
-      </c>
-      <c r="E17" s="39"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="7">
-        <v>43257</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="7">
-        <v>43250</v>
-      </c>
-      <c r="E19" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" s="37">
-        <v>43244</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="35">
-        <v>43250</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="38">
-        <v>43250</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="34">
-        <v>43248</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="38">
-        <v>43261</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="34">
-        <v>43261</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="38">
-        <v>43261</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" s="34">
-        <v>43261</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="C25" s="6">
+        <v>43264</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="38">
-        <v>43261</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="34">
-        <v>43261</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="38">
-        <v>43264</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="12" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>